<commit_message>
small error handling in import inventory
</commit_message>
<xml_diff>
--- a/public/assets/import-inventory.xlsx
+++ b/public/assets/import-inventory.xlsx
@@ -160,23 +160,7 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">12 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">pack</t>
-    </r>
+    <t xml:space="preserve">12 pack</t>
   </si>
   <si>
     <t xml:space="preserve">Meropenem</t>
@@ -206,7 +190,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -260,11 +244,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">

</xml_diff>